<commit_message>
Reorganize docs; remove Invoke-CvadReporting
Move generated command help markdown into docs/docs/CTXCloudApi and update site paths (moved many docs/site pages, updated search index and sitemap). Remove the large Invoke-CvadReporting implementation from the built module (moved original script to Removed/Invoke-CvadReporting.ps1 and deleted embedded region from Output/0.1.33/CTXCloudApi.psm1). Simplify Reports-Colors by removing HKCU bootstrap comments and keeping direct color assignments. Delete generated en-US help XML from Output/0.1.33 and update generated timestamps in PSD1 files; bump Version.json and refresh Issues.md timestamp/contents.
</commit_message>
<xml_diff>
--- a/Issues.xlsx
+++ b/Issues.xlsx
@@ -8,14 +8,14 @@
     <sheet name="Other" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Other'!$A$1:$C$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Other'!$A$1:$C$21</definedName>
   </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Catagory</t>
   </si>
@@ -29,34 +29,64 @@
     <t>External Help</t>
   </si>
   <si>
-    <t>Get-CTXAPI_Machine.md</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_Machine.md - ### -Name - {{ Fill Name Description }}</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md - ## SYNOPSIS - {{ Fill in the Synopsis }}</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md - ## DESCRIPTION - {{ Fill in the Description }}</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md - ```powershell - PS C:\&gt; {{ Add example code here }}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get-CTXAPI_VDAUptime.md -  - {{ Add example description here }}</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md - ### -APIHeader - {{ Fill APIHeader Description }}</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md - ### -Export - {{ Fill Export Description }}</t>
-  </si>
-  <si>
-    <t>Get-CTXAPI_VDAUptime.md - ### -ReportPath - {{ Fill ReportPath Description }}</t>
+    <t>Connect-CTXAPI</t>
+  </si>
+  <si>
+    <t>Did not create the .md file</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_Application</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_CloudService</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_ConfigLog</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_DeliveryGroup</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_Hypervisor</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_LowLevelOperation</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_Machine</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_MachineCatalog</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_MonitorData</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_ResourceLocation</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_Session</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_SiteDetail</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_VDAUptime</t>
+  </si>
+  <si>
+    <t>Get-CTXAPI_Zone</t>
+  </si>
+  <si>
+    <t>New-CTXAPI_Machine</t>
+  </si>
+  <si>
+    <t>New-CTXAPI_Report</t>
+  </si>
+  <si>
+    <t>Set-CTXAPI_MachinePowerState</t>
+  </si>
+  <si>
+    <t>Test-CTXAPI_Header</t>
   </si>
 </sst>
 </file>
@@ -108,7 +138,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" state="frozen" activePane="bottomLeft"/>
@@ -118,8 +148,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.1482801437378" customWidth="1"/>
-    <col min="2" max="2" width="26.2772789001465" customWidth="1"/>
-    <col min="3" max="3" width="72.2681503295898" customWidth="1"/>
+    <col min="2" max="2" width="29.9633808135986" customWidth="1"/>
+    <col min="3" max="3" width="24.4306449890137" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -133,12 +163,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="3">
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>5</v>
@@ -149,10 +190,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -160,10 +201,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -171,10 +212,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -182,10 +223,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -193,10 +234,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -204,10 +245,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -215,14 +256,124 @@
         <v>3</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C10"/>
+  <autoFilter ref="A1:C21"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>